<commit_message>
update DOT hemo paras
</commit_message>
<xml_diff>
--- a/Dataset/DOT_hemo1.xlsx
+++ b/Dataset/DOT_hemo1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mingh\Box\DOT\chemo_US\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565AE2A2-9EE6-48AF-A0DB-E7CAAF8A27C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805284D5-1330-4C95-8A71-A553255FA9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16845" yWindow="480" windowWidth="20400" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17565" yWindow="990" windowWidth="20400" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFDEE97-305A-45CD-A167-9798C730B9E2}">
   <dimension ref="A1:X310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="J302" sqref="J302"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="A311" sqref="A311:E311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,96 +592,96 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>67.739229540830678</v>
+        <v>93.422325043864817</v>
       </c>
       <c r="B2">
-        <v>68.02849173684254</v>
+        <v>89.75599155294401</v>
       </c>
       <c r="C2">
-        <v>64.067958997529033</v>
+        <v>77.06761800207245</v>
       </c>
       <c r="D2">
-        <v>66.190995135208354</v>
+        <v>92.89159298520751</v>
       </c>
       <c r="E2">
-        <v>66.795166547845369</v>
+        <v>88.449563637334634</v>
       </c>
       <c r="F2">
-        <v>68.360439387359392</v>
+        <v>92.133922026468852</v>
       </c>
       <c r="G2">
-        <v>67.647926865720294</v>
+        <v>94.060429651605887</v>
       </c>
       <c r="H2">
-        <v>65.975229974918861</v>
+        <v>99.319244882157207</v>
       </c>
       <c r="I2">
-        <v>66.910529202294597</v>
+        <v>100.79116490368604</v>
       </c>
       <c r="J2">
-        <v>67.652625685061224</v>
+        <v>98.538979573807396</v>
       </c>
       <c r="K2">
-        <v>67.958226448503325</v>
+        <v>96.343327645167562</v>
       </c>
       <c r="L2">
-        <v>68.54847856313323</v>
+        <v>96.352824085283203</v>
       </c>
       <c r="M2">
-        <v>70.659825663785838</v>
+        <v>93.763700113525388</v>
       </c>
       <c r="N2">
-        <v>70.460102611276838</v>
+        <v>96.288294729206811</v>
       </c>
       <c r="O2">
-        <v>69.09321675215061</v>
+        <v>92.155896825640369</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>94.442286980716162</v>
+        <v>84.410955116312536</v>
       </c>
       <c r="B3">
-        <v>90.133665457376978</v>
+        <v>84.980044169608561</v>
       </c>
       <c r="C3">
-        <v>90.727723059602411</v>
+        <v>84.892962167637847</v>
       </c>
       <c r="D3">
-        <v>91.223078054382057</v>
+        <v>84.119296063060801</v>
       </c>
       <c r="E3">
-        <v>89.139511108194213</v>
+        <v>81.950685961203931</v>
       </c>
       <c r="F3">
-        <v>83.39798749297448</v>
+        <v>80.636148785626929</v>
       </c>
       <c r="G3">
-        <v>100.35565680146159</v>
+        <v>86.129849659662227</v>
       </c>
       <c r="H3">
-        <v>104.01235236507706</v>
+        <v>86.575842454432092</v>
       </c>
       <c r="I3">
-        <v>98.871658573933047</v>
+        <v>86.869070257475357</v>
       </c>
       <c r="J3">
-        <v>98.698877605655653</v>
+        <v>86.467839812850585</v>
       </c>
       <c r="K3">
-        <v>97.547932351484604</v>
+        <v>85.210990466618227</v>
       </c>
       <c r="L3">
-        <v>94.605530769552445</v>
+        <v>82.782085057671594</v>
       </c>
       <c r="M3">
-        <v>94.149386889800951</v>
+        <v>83.321613885378952</v>
       </c>
       <c r="N3">
-        <v>93.91556152111859</v>
+        <v>83.307252191624116</v>
       </c>
       <c r="O3">
-        <v>95.413095679412024</v>
+        <v>84.509690695524512</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1554,31 +1554,10 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>24.996798811594978</v>
+        <v>94.48097819510545</v>
       </c>
       <c r="B37">
-        <v>44.633343318970205</v>
-      </c>
-      <c r="C37">
-        <v>22.6093654058844</v>
-      </c>
-      <c r="D37">
-        <v>19.328110241808208</v>
-      </c>
-      <c r="E37">
-        <v>21.7979031943539</v>
-      </c>
-      <c r="F37">
-        <v>20.852556700546927</v>
-      </c>
-      <c r="G37">
-        <v>23.50379045667173</v>
-      </c>
-      <c r="H37">
-        <v>22.53368074007442</v>
-      </c>
-      <c r="I37">
-        <v>24.71564043445003</v>
+        <v>94.48097819510545</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -2527,31 +2506,31 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>64.192000501004912</v>
+        <v>78.762445800138238</v>
       </c>
       <c r="B72">
-        <v>60.989257778230098</v>
+        <v>73.216551677283277</v>
       </c>
       <c r="C72">
-        <v>65.52158523166743</v>
+        <v>82.823721938382533</v>
       </c>
       <c r="D72">
-        <v>65.573644462231599</v>
+        <v>78.376648595400525</v>
       </c>
       <c r="E72">
-        <v>65.321236678734024</v>
+        <v>79.482256486819409</v>
       </c>
       <c r="F72">
-        <v>65.275921844118997</v>
+        <v>79.015170564324691</v>
       </c>
       <c r="G72">
-        <v>64.65477930656742</v>
+        <v>81.908619796671488</v>
       </c>
       <c r="H72">
-        <v>63.625533475723692</v>
+        <v>78.633430139666046</v>
       </c>
       <c r="I72">
-        <v>62.574045230766082</v>
+        <v>76.643167202557933</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -3179,25 +3158,25 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>147.92676231044996</v>
+        <v>102.1879871806351</v>
       </c>
       <c r="B99">
-        <v>144.28141114429434</v>
+        <v>99.273252401867197</v>
       </c>
       <c r="C99">
-        <v>139.26029957218876</v>
+        <v>102.94670584891755</v>
       </c>
       <c r="D99">
-        <v>144.77986603967997</v>
+        <v>100.81354095372939</v>
       </c>
       <c r="E99">
-        <v>167.27835609409638</v>
+        <v>107.74235068693692</v>
       </c>
       <c r="F99">
-        <v>145.00105621423342</v>
+        <v>107.33293116046683</v>
       </c>
       <c r="G99">
-        <v>146.95958479820695</v>
+        <v>95.01914203189277</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -4267,37 +4246,37 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>106.90869565855512</v>
+        <v>79.607376614078248</v>
       </c>
       <c r="B145">
-        <v>89.753339313680002</v>
+        <v>78.452992997065834</v>
       </c>
       <c r="C145">
-        <v>90.139907374038785</v>
+        <v>79.370936261222212</v>
       </c>
       <c r="D145">
-        <v>101.57810672202349</v>
+        <v>82.314730720007688</v>
       </c>
       <c r="E145">
-        <v>110.09950102744121</v>
+        <v>78.872305113372377</v>
       </c>
       <c r="F145">
-        <v>106.96986746241654</v>
+        <v>78.657189768593369</v>
       </c>
       <c r="G145">
-        <v>108.97998099681392</v>
+        <v>79.094799427178941</v>
       </c>
       <c r="H145">
-        <v>113.23640852400246</v>
+        <v>80.032482406943998</v>
       </c>
       <c r="I145">
-        <v>115.24906837525248</v>
+        <v>79.747366398041635</v>
       </c>
       <c r="J145">
-        <v>115.55380059432258</v>
+        <v>79.301625763411181</v>
       </c>
       <c r="K145">
-        <v>117.52697619555997</v>
+        <v>80.229337284945302</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
@@ -5347,46 +5326,19 @@
     </row>
     <row r="179" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>20.533317985467104</v>
+        <v>52.033332622334058</v>
       </c>
       <c r="B179">
-        <v>15.689278352865276</v>
+        <v>55.60332467579412</v>
       </c>
       <c r="C179">
-        <v>14.646539542471695</v>
+        <v>55.214124902571385</v>
       </c>
       <c r="D179">
-        <v>11.858683005155802</v>
+        <v>48.556026108449281</v>
       </c>
       <c r="E179">
-        <v>14.597079417891059</v>
-      </c>
-      <c r="F179">
-        <v>12.89815258448837</v>
-      </c>
-      <c r="G179">
-        <v>13.978880964651575</v>
-      </c>
-      <c r="H179">
-        <v>16.914241278556521</v>
-      </c>
-      <c r="I179">
-        <v>15.275180972044499</v>
-      </c>
-      <c r="J179">
-        <v>28.09605160580027</v>
-      </c>
-      <c r="K179">
-        <v>20.045323525350749</v>
-      </c>
-      <c r="L179">
-        <v>28.228258420019792</v>
-      </c>
-      <c r="M179">
-        <v>34.372799640398476</v>
-      </c>
-      <c r="N179">
-        <v>40.332664501378332</v>
+        <v>48.759854802521424</v>
       </c>
     </row>
     <row r="180" spans="1:24" x14ac:dyDescent="0.25">
@@ -9063,21 +9015,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F44A64374FD3D14CB564863B3B8E6093" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="694d0147b22a524c25d3e435aa7240dc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="da119f74-4cb9-42fc-a8eb-fc471a42e731" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77310024378a84fe98cc6cea8372974f" ns3:_="">
     <xsd:import namespace="da119f74-4cb9-42fc-a8eb-fc471a42e731"/>
@@ -9259,31 +9196,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2431487B-7AA1-4387-9AC3-40F40733A036}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="da119f74-4cb9-42fc-a8eb-fc471a42e731"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFBFDD7C-7266-4202-BA80-31F89B71E939}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F5BA874-E0DC-48CB-AB02-950BA1AAC79E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9299,4 +9227,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFBFDD7C-7266-4202-BA80-31F89B71E939}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2431487B-7AA1-4387-9AC3-40F40733A036}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="da119f74-4cb9-42fc-a8eb-fc471a42e731"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>